<commit_message>
corrections for new lines in xls and tests
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -154,10 +154,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -188,15 +188,20 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="str">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("FORM", "ULA")</f>
         <v>FORMULA</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B4" s="0" t="n">
         <f aca="false">1+2</f>
         <v>3</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C4" s="0" t="n">
         <v>2.1</v>
       </c>
     </row>
@@ -219,7 +224,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="1" sqref="3:3 E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
adds consistency between unit tests, handles trailing field delimiters
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Row1Cell1</t>
   </si>
@@ -157,7 +157,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="3:3"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -180,9 +180,7 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
@@ -224,7 +222,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="1" sqref="3:3 E15"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fix spreadsheet errors in file (ie re-save in excel)
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthew.cockayne/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ian.dunlop/IdeaProjects/consumer-spreadsheetconverter/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2B0E63-4328-244B-A78F-2598EF722405}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{63AB60CE-1146-F047-B6D5-2CFCB8D169CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="41120" windowHeight="21920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -102,9 +107,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,7 +426,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -442,18 +446,12 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="str">

</xml_diff>